<commit_message>
more trials for eval 3
</commit_message>
<xml_diff>
--- a/data/AB_Data+Table.xlsx
+++ b/data/AB_Data+Table.xlsx
@@ -2,19 +2,23 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26606"/>
-  <workbookPr/>
+  <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/francesshapiro/Desktop/cs182-finalproject/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1600" yWindow="460" windowWidth="27960" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="1760" yWindow="460" windowWidth="27960" windowHeight="17540" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
+  <pivotCaches>
+    <pivotCache cacheId="5" r:id="rId3"/>
+  </pivotCaches>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -24,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="28">
   <si>
     <t>Number of Teams</t>
   </si>
@@ -100,15 +104,31 @@
   <si>
     <t>Team 1</t>
   </si>
+  <si>
+    <t>Column Labels</t>
+  </si>
+  <si>
+    <t>Row Labels</t>
+  </si>
+  <si>
+    <t>Grand Total</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -121,15 +141,20 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -137,19 +162,459 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Accent5" xfId="1" builtinId="45"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="28">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color theme="0"/>
+        </vertical>
+        <horizontal style="thin">
+          <color theme="0"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical style="thin">
+          <color theme="0"/>
+        </vertical>
+        <horizontal style="thin">
+          <color theme="0"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical style="thin">
+          <color theme="0"/>
+        </vertical>
+        <horizontal style="thin">
+          <color theme="0"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color theme="0"/>
+        </vertical>
+        <horizontal style="thin">
+          <color theme="0"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical style="thin">
+          <color theme="0"/>
+        </vertical>
+        <horizontal style="thin">
+          <color theme="0"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical style="thin">
+          <color theme="0"/>
+        </vertical>
+        <horizontal style="thin">
+          <color theme="0"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color theme="0"/>
+        </vertical>
+        <horizontal style="thin">
+          <color theme="0"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical style="thin">
+          <color theme="0"/>
+        </vertical>
+        <horizontal style="thin">
+          <color theme="0"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical style="thin">
+          <color theme="0"/>
+        </vertical>
+        <horizontal style="thin">
+          <color theme="0"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color theme="0"/>
+        </vertical>
+        <horizontal style="thin">
+          <color theme="0"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical style="thin">
+          <color theme="0"/>
+        </vertical>
+        <horizontal style="thin">
+          <color theme="0"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical style="thin">
+          <color theme="0"/>
+        </vertical>
+        <horizontal style="thin">
+          <color theme="0"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color theme="0"/>
+        </vertical>
+        <horizontal style="thin">
+          <color theme="0"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical style="thin">
+          <color theme="0"/>
+        </vertical>
+        <horizontal style="thin">
+          <color theme="0"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color theme="0"/>
+        </right>
+        <top style="thin">
+          <color theme="0"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical style="thin">
+          <color theme="0"/>
+        </vertical>
+        <horizontal style="thin">
+          <color theme="0"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -157,6 +622,306 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12382500" y="2235200"/>
+          <a:ext cx="4965700" cy="622300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12382500" y="2997200"/>
+          <a:ext cx="4965700" cy="622300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Microsoft Office User" refreshedDate="43073.536623495369" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="1">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="W21:AJ22" sheet="Sheet1"/>
+  </cacheSource>
+  <cacheFields count="14">
+    <cacheField name="Team 0" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="201" maxValue="201" count="1">
+        <n v="201"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Team 1" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="95" maxValue="95" count="1">
+        <n v="95"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Team 02" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="53.44" maxValue="53.44"/>
+    </cacheField>
+    <cacheField name="Team 12" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="50.73" maxValue="50.73"/>
+    </cacheField>
+    <cacheField name="Team 03" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="21.27" maxValue="21.27"/>
+    </cacheField>
+    <cacheField name="Team 13" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="14.62" maxValue="14.62"/>
+    </cacheField>
+    <cacheField name="Team 04" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="53" maxValue="53"/>
+    </cacheField>
+    <cacheField name="Team 14" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="52" maxValue="52"/>
+    </cacheField>
+    <cacheField name="Team 05" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="12903" maxValue="12903"/>
+    </cacheField>
+    <cacheField name="Team 15" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="7859" maxValue="7859"/>
+    </cacheField>
+    <cacheField name="Team 06" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="43.01" maxValue="43.01"/>
+    </cacheField>
+    <cacheField name="Team 16" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="26.2" maxValue="26.2"/>
+    </cacheField>
+    <cacheField name="Team 07" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="38.82" maxValue="38.82"/>
+    </cacheField>
+    <cacheField name="Team 17" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="29.45" maxValue="29.45"/>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="1">
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="53.44"/>
+    <n v="50.73"/>
+    <n v="21.27"/>
+    <n v="14.62"/>
+    <n v="53"/>
+    <n v="52"/>
+    <n v="12903"/>
+    <n v="7859"/>
+    <n v="43.01"/>
+    <n v="26.2"/>
+    <n v="38.82"/>
+    <n v="29.45"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:C6" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="14">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="2">
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="2">
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="1"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <pivotTableStyleInfo name="PivotStyleMedium7" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="J25:K26" totalsRowShown="0" headerRowDxfId="20" dataDxfId="27">
+  <autoFilter ref="J25:K26"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="Team 0" dataDxfId="22"/>
+    <tableColumn id="2" name="Team 1" dataDxfId="21"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table8" displayName="Table8" ref="K20:L21" totalsRowShown="0" headerRowDxfId="17" dataDxfId="26">
+  <autoFilter ref="K20:L21"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="Team 0" dataDxfId="19"/>
+    <tableColumn id="2" name="Team 1" dataDxfId="18"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table9" displayName="Table9" ref="M20:N21" totalsRowShown="0" headerRowDxfId="14" dataDxfId="25">
+  <autoFilter ref="M20:N21"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="Team 0" dataDxfId="16"/>
+    <tableColumn id="2" name="Team 1" dataDxfId="15"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table10" displayName="Table10" ref="N8:O9" totalsRowShown="0" headerRowDxfId="11" dataDxfId="24">
+  <autoFilter ref="N8:O9"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="Team 0" dataDxfId="13"/>
+    <tableColumn id="2" name="Team 1" dataDxfId="12"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table11" displayName="Table11" ref="L25:M26" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="L25:M26"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="Team 0" dataDxfId="7"/>
+    <tableColumn id="2" name="Team 1" dataDxfId="6"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Table12" displayName="Table12" ref="N25:O26" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+  <autoFilter ref="N25:O26"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="Team 0" dataDxfId="3"/>
+    <tableColumn id="2" name="Team 1" dataDxfId="2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="Table13" displayName="Table13" ref="O20:P21" totalsRowShown="0" headerRowDxfId="8" dataDxfId="23">
+  <autoFilter ref="O20:P21"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="Team 0" dataDxfId="10"/>
+    <tableColumn id="2" name="Team 1" dataDxfId="9"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -422,15 +1187,61 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V302"/>
+  <dimension ref="A3:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="U25" sqref="U25"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B3" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4">
+        <v>95</v>
+      </c>
+      <c r="C4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="4">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P302"/>
+  <sheetViews>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="L29" sqref="L29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -447,7 +1258,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>2</v>
       </c>
@@ -474,7 +1285,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -503,7 +1314,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -524,7 +1335,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>2</v>
       </c>
@@ -556,7 +1367,7 @@
         <v>21.273684210526316</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>2</v>
       </c>
@@ -588,7 +1399,7 @@
         <v>14.618811881188119</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>2</v>
       </c>
@@ -608,8 +1419,12 @@
         <f t="shared" si="0"/>
         <v>68</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="N7" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="O7" s="6"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>2</v>
       </c>
@@ -636,8 +1451,14 @@
         <f>MEDIAN(D2:D203)</f>
         <v>53</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="N8" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="O8" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>2</v>
       </c>
@@ -664,8 +1485,14 @@
         <f>MEDIAN(D204:D298)</f>
         <v>52</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="N9" s="5">
+        <v>53</v>
+      </c>
+      <c r="O9" s="5">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>2</v>
       </c>
@@ -686,7 +1513,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>2</v>
       </c>
@@ -718,7 +1545,7 @@
         <v>43.01</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>2</v>
       </c>
@@ -750,7 +1577,7 @@
         <v>26.196666666666665</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>2</v>
       </c>
@@ -771,7 +1598,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>2</v>
       </c>
@@ -799,7 +1626,7 @@
         <v>38.821782178217823</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>2</v>
       </c>
@@ -827,7 +1654,7 @@
         <v>29.452631578947368</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>2</v>
       </c>
@@ -848,7 +1675,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>2</v>
       </c>
@@ -869,7 +1696,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>2</v>
       </c>
@@ -890,7 +1717,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>2</v>
       </c>
@@ -910,29 +1737,20 @@
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="I19" t="s">
-        <v>16</v>
-      </c>
-      <c r="K19" t="s">
+      <c r="K19" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="M19" t="s">
+      <c r="L19" s="6"/>
+      <c r="M19" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="O19" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q19" t="s">
-        <v>20</v>
-      </c>
-      <c r="S19" t="s">
-        <v>21</v>
-      </c>
-      <c r="U19" t="s">
+      <c r="N19" s="6"/>
+      <c r="O19" s="6" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="P19" s="6"/>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>2</v>
       </c>
@@ -952,50 +1770,26 @@
         <f t="shared" si="0"/>
         <v>47</v>
       </c>
-      <c r="I20" t="s">
+      <c r="K20" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="J20" t="s">
+      <c r="L20" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="K20" t="s">
+      <c r="M20" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="L20" t="s">
+      <c r="N20" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="M20" t="s">
+      <c r="O20" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="N20" t="s">
+      <c r="P20" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="O20" t="s">
-        <v>23</v>
-      </c>
-      <c r="P20" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q20" t="s">
-        <v>23</v>
-      </c>
-      <c r="R20" t="s">
-        <v>24</v>
-      </c>
-      <c r="S20" t="s">
-        <v>23</v>
-      </c>
-      <c r="T20" t="s">
-        <v>24</v>
-      </c>
-      <c r="U20" t="s">
-        <v>23</v>
-      </c>
-      <c r="V20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>2</v>
       </c>
@@ -1015,50 +1809,26 @@
         <f t="shared" si="0"/>
         <v>71</v>
       </c>
-      <c r="I21">
-        <v>201</v>
-      </c>
-      <c r="J21">
-        <v>95</v>
-      </c>
-      <c r="K21">
+      <c r="K21" s="5">
         <v>53.44</v>
       </c>
-      <c r="L21">
+      <c r="L21" s="5">
         <v>50.73</v>
       </c>
-      <c r="M21">
+      <c r="M21" s="5">
         <v>21.27</v>
       </c>
-      <c r="N21">
+      <c r="N21" s="5">
         <v>14.62</v>
       </c>
-      <c r="O21">
-        <v>53</v>
-      </c>
-      <c r="P21">
-        <v>52</v>
-      </c>
-      <c r="Q21">
-        <v>12903</v>
-      </c>
-      <c r="R21">
-        <v>7859</v>
-      </c>
-      <c r="S21">
-        <v>43.01</v>
-      </c>
-      <c r="T21">
-        <v>26.2</v>
-      </c>
-      <c r="U21">
+      <c r="O21" s="5">
         <v>38.82</v>
       </c>
-      <c r="V21">
+      <c r="P21" s="5">
         <v>29.45</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>2</v>
       </c>
@@ -1079,7 +1849,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>2</v>
       </c>
@@ -1100,7 +1870,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>2</v>
       </c>
@@ -1120,8 +1890,20 @@
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="J24" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="K24" s="6"/>
+      <c r="L24" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="M24" s="6"/>
+      <c r="N24" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="O24" s="6"/>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>2</v>
       </c>
@@ -1141,8 +1923,26 @@
         <f t="shared" si="0"/>
         <v>59</v>
       </c>
-    </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="J25" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="K25" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="L25" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="M25" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="N25" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="O25" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>2</v>
       </c>
@@ -1162,8 +1962,26 @@
         <f t="shared" si="0"/>
         <v>47</v>
       </c>
-    </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="J26" s="5">
+        <v>201</v>
+      </c>
+      <c r="K26" s="5">
+        <v>95</v>
+      </c>
+      <c r="L26" s="5">
+        <v>12903</v>
+      </c>
+      <c r="M26" s="5">
+        <v>7859</v>
+      </c>
+      <c r="N26" s="5">
+        <v>43.01</v>
+      </c>
+      <c r="O26" s="5">
+        <v>26.2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>2</v>
       </c>
@@ -1184,7 +2002,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>2</v>
       </c>
@@ -1205,7 +2023,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>2</v>
       </c>
@@ -1226,7 +2044,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>2</v>
       </c>
@@ -1247,7 +2065,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>2</v>
       </c>
@@ -1268,7 +2086,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>2</v>
       </c>
@@ -6963,7 +7781,26 @@
   <sortState ref="A2:E302">
     <sortCondition ref="C2:C302"/>
   </sortState>
+  <mergeCells count="7">
+    <mergeCell ref="O19:P19"/>
+    <mergeCell ref="J24:K24"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="M19:N19"/>
+    <mergeCell ref="N7:O7"/>
+    <mergeCell ref="L24:M24"/>
+    <mergeCell ref="N24:O24"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <drawing r:id="rId1"/>
+  <tableParts count="7">
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
+    <tablePart r:id="rId6"/>
+    <tablePart r:id="rId7"/>
+    <tablePart r:id="rId8"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>